<commit_message>
Testing et référencement des bugs
</commit_message>
<xml_diff>
--- a/doc/protocole_de_tests.xlsx
+++ b/doc/protocole_de_tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\HEG - Intranet\01-Semestre 1\630-Technologies informatiques\631-1 Fondement de la programmation\Projet_Prog\ProjetProg1IGPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\HEG - Intranet\01-Semestre 1\630-Technologies informatiques\631-1 Fondement de la programmation\Projet_Prog\ProjetProg1IGPT\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>Tests</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Rendre livre emprunté</t>
   </si>
   <si>
-    <t>Rendre livre non emprunté</t>
-  </si>
-  <si>
     <t>Rendre livre qui n'existe pas</t>
   </si>
   <si>
@@ -81,6 +78,129 @@
   </si>
   <si>
     <t>KO</t>
+  </si>
+  <si>
+    <t>Numéro ISBN déjà existant (+1 exemplaire ou alors erreur ?)</t>
+  </si>
+  <si>
+    <t>Saisie  d'un Nombre d'exemplaire négatifs</t>
+  </si>
+  <si>
+    <t>Saisie d'un Nombre de pages négatifs</t>
+  </si>
+  <si>
+    <t>Ajout d'un livre</t>
+  </si>
+  <si>
+    <t>5. Ajout d'un exemplaire d'un livre</t>
+  </si>
+  <si>
+    <t>Ajout d'un exemplaire</t>
+  </si>
+  <si>
+    <t>ISBN invalide</t>
+  </si>
+  <si>
+    <t>6. Ajouter nouvel adherent</t>
+  </si>
+  <si>
+    <t>Code adherent qui n'existe pas</t>
+  </si>
+  <si>
+    <t>Code adherent qui existe déjà</t>
+  </si>
+  <si>
+    <t>Ajout adherent</t>
+  </si>
+  <si>
+    <t>7. Recherche et affichage de livre(s)</t>
+  </si>
+  <si>
+    <t>ISBN qui n'existe pas</t>
+  </si>
+  <si>
+    <t>Recherche livre</t>
+  </si>
+  <si>
+    <t>Fonction continuer / arrêter</t>
+  </si>
+  <si>
+    <t>8. Recherche et affichage d'emprunts</t>
+  </si>
+  <si>
+    <t>Emprunts non trouvé</t>
+  </si>
+  <si>
+    <t>Recherche emprunt</t>
+  </si>
+  <si>
+    <t>Compteur num emprunts</t>
+  </si>
+  <si>
+    <t>9. Recherhce et affichage d'adherent</t>
+  </si>
+  <si>
+    <t>Recherche adherent</t>
+  </si>
+  <si>
+    <t>Code invalide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10. Supprimer exemplaire livre </t>
+  </si>
+  <si>
+    <t>Supression exemplaire</t>
+  </si>
+  <si>
+    <t>Si livre existe pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si exemplaire = 0 (Suppression livre de la biblio) ? </t>
+  </si>
+  <si>
+    <t>11. Supprimer livre</t>
+  </si>
+  <si>
+    <t>Supression livre en entier y compris tous ses exemplaires</t>
+  </si>
+  <si>
+    <t>12.  Supprimer adherent</t>
+  </si>
+  <si>
+    <t>Suppression adherent</t>
+  </si>
+  <si>
+    <t>Afficher message clair si il a encore des emprunts</t>
+  </si>
+  <si>
+    <t>Empécher la suppression si encore emprunts</t>
+  </si>
+  <si>
+    <t>13 Vérifier si biliothèque est ouverte</t>
+  </si>
+  <si>
+    <t>Jours ouvert et Heure ouvert --&gt; Ouvert</t>
+  </si>
+  <si>
+    <t>Jours ouvert et heure fermée --&gt; Fermé</t>
+  </si>
+  <si>
+    <t>Jours fermé et heure ouvert --&gt; Fermé</t>
+  </si>
+  <si>
+    <t>Jour fermé et heure fermé --&gt; Fermé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour invalide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">heure invalide </t>
+  </si>
+  <si>
+    <t>Lundi 19h --&gt; Ouvert</t>
+  </si>
+  <si>
+    <t>Minuscule Majuscule jour de la semaine</t>
   </si>
 </sst>
 </file>
@@ -123,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -131,28 +251,153 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -171,6 +416,69 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -484,133 +792,573 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A39" sqref="A39:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.921875" customWidth="1"/>
-    <col min="2" max="2" width="35.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.07421875" style="5"/>
+    <col min="2" max="2" width="50.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.07421875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="8"/>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="8"/>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="8"/>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="9"/>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="7"/>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="7"/>
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="8"/>
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="7"/>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="8"/>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="8"/>
+      <c r="B19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" s="9"/>
+      <c r="B20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" s="7"/>
+      <c r="B22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" s="9"/>
+      <c r="B23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="7"/>
+      <c r="B25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" s="9"/>
+      <c r="B26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" s="7"/>
+      <c r="B28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" s="8"/>
+      <c r="B29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" s="9"/>
+      <c r="B30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" s="7"/>
+      <c r="B32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" s="8"/>
+      <c r="B33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" s="9"/>
+      <c r="B34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" s="7"/>
+      <c r="B36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A37" s="8"/>
+      <c r="B37" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" s="9"/>
+      <c r="B38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="16"/>
+      <c r="C39" s="17"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" s="7"/>
+      <c r="B40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" s="8"/>
+      <c r="B41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" s="9"/>
+      <c r="B42" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" s="7"/>
+      <c r="B44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" s="9"/>
+      <c r="B45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" s="7"/>
+      <c r="B47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" s="8"/>
+      <c r="B48" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" s="8"/>
+      <c r="B49" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" s="9"/>
+      <c r="B50" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A52" s="7"/>
+      <c r="B52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A53" s="8"/>
+      <c r="B53" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" s="8"/>
+      <c r="B54" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" s="8"/>
+      <c r="B55" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" s="8"/>
+      <c r="B56" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" s="8"/>
+      <c r="B57" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A58" s="8"/>
+      <c r="B58" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59" s="9"/>
+      <c r="B59" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <mergeCells count="24">
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C1 C34 C38 C3:C8 C10:C11 C13:C15 C17:C20 C22:C23 C25:C26 C28:C30 C32 C36 C40:C1048576">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"KO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modification mise en page - protocole de tests
</commit_message>
<xml_diff>
--- a/doc/protocole_de_tests.xlsx
+++ b/doc/protocole_de_tests.xlsx
@@ -344,16 +344,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -375,13 +371,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -806,512 +805,513 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="9"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" s="9"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27" s="15" t="s">
+      <c r="C26" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="9"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" s="15" t="s">
+      <c r="C30" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" s="9"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" s="15" t="s">
+      <c r="C34" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" s="7"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="5"/>
+      <c r="B36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" s="9"/>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A39" s="15" t="s">
+      <c r="C38" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" s="7"/>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="5"/>
+      <c r="B40" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" s="8"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" s="9"/>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="4"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" s="7"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="5"/>
+      <c r="B44" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" s="9"/>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="7"/>
+      <c r="B45" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A47" s="7"/>
-      <c r="B47" s="5" t="s">
+      <c r="A47" s="5"/>
+      <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A48" s="8"/>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A49" s="8"/>
-      <c r="B49" s="5" t="s">
+      <c r="A49" s="6"/>
+      <c r="B49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A50" s="9"/>
-      <c r="B50" s="5" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="4"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" s="7"/>
-      <c r="B52" s="5" t="s">
+      <c r="A52" s="5"/>
+      <c r="B52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" s="8"/>
-      <c r="B53" s="5" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="5" t="s">
+      <c r="A54" s="6"/>
+      <c r="B54" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="5" t="s">
+      <c r="A55" s="6"/>
+      <c r="B55" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="5" t="s">
+      <c r="A56" s="6"/>
+      <c r="B56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" s="8"/>
-      <c r="B57" s="5" t="s">
+      <c r="A57" s="6"/>
+      <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" s="8"/>
-      <c r="B58" s="5" t="s">
+      <c r="A58" s="6"/>
+      <c r="B58" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" s="9"/>
-      <c r="B59" s="5" t="s">
+      <c r="A59" s="7"/>
+      <c r="B59" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="4" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="27">
+    <mergeCell ref="A51:C51"/>
     <mergeCell ref="A52:A59"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:C2"/>
@@ -1330,6 +1330,8 @@
     <mergeCell ref="A47:A50"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A46:C46"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A13:A15"/>
@@ -1337,7 +1339,7 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A25:A26"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1 C34 C38 C3:C8 C10:C11 C13:C15 C17:C20 C22:C23 C25:C26 C28:C30 C32 C36 C40:C1048576">
+  <conditionalFormatting sqref="C1 C34 C38 C3:C8 C10:C11 C13:C15 C17:C20 C22:C23 C25:C26 C28:C30 C32 C36 C40:C42 C44:C45 C47:C50 C52:C1048576">
     <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"KO"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Petite modification - correction de bugs
</commit_message>
<xml_diff>
--- a/doc/protocole_de_tests.xlsx
+++ b/doc/protocole_de_tests.xlsx
@@ -356,6 +356,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,9 +373,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -379,66 +382,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -793,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -805,23 +753,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="5"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -830,7 +778,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -839,7 +787,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -848,7 +796,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="6"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -857,7 +805,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
@@ -866,7 +814,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="7"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
@@ -875,14 +823,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -891,7 +839,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -900,14 +848,14 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -916,7 +864,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -925,7 +873,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -934,14 +882,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
@@ -950,7 +898,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="6"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
@@ -959,7 +907,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="6"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -968,7 +916,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
@@ -977,14 +925,14 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="5"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
@@ -993,7 +941,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1002,14 +950,14 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="5"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="3" t="s">
         <v>27</v>
       </c>
@@ -1018,7 +966,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1026,15 +974,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28" s="5"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
@@ -1043,7 +991,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" s="6"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
@@ -1052,7 +1000,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>32</v>
       </c>
@@ -1060,15 +1008,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="5"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="3" t="s">
         <v>35</v>
       </c>
@@ -1077,7 +1025,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="6"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="3" t="s">
         <v>32</v>
       </c>
@@ -1086,7 +1034,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="3" t="s">
         <v>34</v>
       </c>
@@ -1094,15 +1042,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" s="5"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="3" t="s">
         <v>38</v>
       </c>
@@ -1111,7 +1059,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" s="6"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="3" t="s">
         <v>32</v>
       </c>
@@ -1120,7 +1068,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" s="7"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="3" t="s">
         <v>39</v>
       </c>
@@ -1128,15 +1076,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="13" t="s">
+    <row r="39" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" s="5"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1145,7 +1093,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" s="6"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="3" t="s">
         <v>42</v>
       </c>
@@ -1154,7 +1102,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" s="7"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="3" t="s">
         <v>43</v>
       </c>
@@ -1163,14 +1111,14 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" s="5"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="3" t="s">
         <v>45</v>
       </c>
@@ -1179,7 +1127,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" s="7"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="3" t="s">
         <v>42</v>
       </c>
@@ -1188,23 +1136,23 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A47" s="5"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A48" s="6"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="3" t="s">
         <v>26</v>
       </c>
@@ -1213,7 +1161,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A49" s="6"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="3" t="s">
         <v>49</v>
       </c>
@@ -1222,7 +1170,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A50" s="7"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
         <v>48</v>
       </c>
@@ -1231,14 +1179,14 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" s="5"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="3" t="s">
         <v>51</v>
       </c>
@@ -1247,7 +1195,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" s="6"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="3" t="s">
         <v>52</v>
       </c>
@@ -1256,7 +1204,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" s="6"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="3" t="s">
         <v>53</v>
       </c>
@@ -1265,7 +1213,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A55" s="6"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="3" t="s">
         <v>54</v>
       </c>
@@ -1274,7 +1222,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" s="6"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="3" t="s">
         <v>57</v>
       </c>
@@ -1283,7 +1231,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" s="6"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="3" t="s">
         <v>55</v>
       </c>
@@ -1292,7 +1240,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" s="6"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="3" t="s">
         <v>56</v>
       </c>
@@ -1301,7 +1249,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" s="7"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="3" t="s">
         <v>58</v>
       </c>
@@ -1311,6 +1259,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A46:C46"/>
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A52:A59"/>
     <mergeCell ref="A1:B1"/>
@@ -1327,39 +1286,28 @@
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <conditionalFormatting sqref="C1 C34 C38 C3:C8 C10:C11 C13:C15 C17:C20 C22:C23 C25:C26 C28:C30 C32 C36 C40:C42 C44:C45 C47:C50 C52:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"KO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correction ajout d'un livre pour empécher de saisir un nombre de page et d'exemplaire négatif
</commit_message>
<xml_diff>
--- a/doc/protocole_de_tests.xlsx
+++ b/doc/protocole_de_tests.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\HEG - Intranet\01-Semestre 1\630-Technologies informatiques\631-1 Fondement de la programmation\Projet_Prog\ProjetProg1IGPT\doc\"/>
@@ -80,9 +80,6 @@
     <t>KO</t>
   </si>
   <si>
-    <t>Numéro ISBN déjà existant (+1 exemplaire ou alors erreur ?)</t>
-  </si>
-  <si>
     <t>Saisie  d'un Nombre d'exemplaire négatifs</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>Minuscule Majuscule jour de la semaine</t>
+  </si>
+  <si>
+    <t>Numéro ISBN déjà existant (--&gt; erreur)</t>
   </si>
 </sst>
 </file>
@@ -359,15 +359,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -377,11 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:C43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -753,23 +753,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -778,7 +778,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -787,7 +787,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -796,7 +796,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -805,16 +805,16 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="7"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
@@ -823,14 +823,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" s="6"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -839,7 +839,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -848,14 +848,14 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" s="6"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
@@ -864,7 +864,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -873,7 +873,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -882,376 +882,376 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17" s="6"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="8"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="10"/>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" s="11"/>
+      <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" s="12" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" s="9"/>
+      <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22" s="6"/>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" s="11"/>
+      <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25" s="6"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26" s="7"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" s="10"/>
+      <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A28" s="6"/>
-      <c r="B28" s="3" t="s">
+      <c r="C29" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" s="11"/>
+      <c r="B30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A30" s="7"/>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="9" t="s">
+      <c r="B31" s="15"/>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" s="9"/>
+      <c r="B32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" s="10"/>
+      <c r="B33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" s="11"/>
+      <c r="B34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A32" s="6"/>
-      <c r="B32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" s="7"/>
-      <c r="B34" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C34" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" s="9"/>
+      <c r="B36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" s="6"/>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A37" s="10"/>
+      <c r="B37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" s="11"/>
+      <c r="B38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" s="7"/>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="9" t="s">
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" s="9"/>
+      <c r="B40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A40" s="6"/>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" s="10"/>
+      <c r="B41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A41" s="8"/>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" s="11"/>
+      <c r="B42" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A42" s="7"/>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A43" s="12" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" s="9"/>
+      <c r="B44" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="14"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A44" s="6"/>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" s="11"/>
+      <c r="B45" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A45" s="7"/>
-      <c r="B45" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A46" s="12" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" s="9"/>
+      <c r="B47" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A47" s="6"/>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" s="10"/>
+      <c r="B48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" s="10"/>
+      <c r="B49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" s="11"/>
+      <c r="B50" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A48" s="8"/>
-      <c r="B48" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A49" s="8"/>
-      <c r="B49" s="3" t="s">
+      <c r="C50" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A50" s="7"/>
-      <c r="B50" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A51" s="12" t="s">
+      <c r="B51" s="7"/>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A52" s="9"/>
+      <c r="B52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A53" s="10"/>
+      <c r="B53" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A53" s="8"/>
-      <c r="B53" s="3" t="s">
+      <c r="C53" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" s="10"/>
+      <c r="B54" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" s="10"/>
+      <c r="B55" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" s="10"/>
+      <c r="B56" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" s="10"/>
+      <c r="B57" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="3" t="s">
+      <c r="C57" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A58" s="10"/>
+      <c r="B58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59" s="11"/>
+      <c r="B59" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A57" s="8"/>
-      <c r="B57" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A58" s="8"/>
-      <c r="B58" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A59" s="7"/>
-      <c r="B59" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>17</v>
@@ -1259,6 +1259,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A46:C46"/>
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A52:A59"/>
     <mergeCell ref="A1:B1"/>
@@ -1275,17 +1286,6 @@
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <conditionalFormatting sqref="C1 C34 C38 C3:C8 C10:C11 C13:C15 C17:C20 C22:C23 C25:C26 C28:C30 C32 C36 C40:C42 C44:C45 C47:C50 C52:C1048576">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">

</xml_diff>

<commit_message>
Modification pour pouvoir saisir le jour de la semaine tant en minuscule que en majuscule
</commit_message>
<xml_diff>
--- a/doc/protocole_de_tests.xlsx
+++ b/doc/protocole_de_tests.xlsx
@@ -742,7 +742,7 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1254,7 +1254,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour du protocole de test
</commit_message>
<xml_diff>
--- a/doc/protocole_de_tests.xlsx
+++ b/doc/protocole_de_tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
   <si>
     <t>Tests</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Numéro ISBN déjà existant (--&gt; erreur)</t>
+  </si>
+  <si>
+    <t>Ok</t>
   </si>
 </sst>
 </file>
@@ -742,7 +745,7 @@
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -819,7 +822,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>